<commit_message>
correct auto/manual column in ga spreadsheet
</commit_message>
<xml_diff>
--- a/startup/xlsx/glancing_angle.xlsx
+++ b/startup/xlsx/glancing_angle.xlsx
@@ -25,7 +25,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -117,7 +117,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -209,7 +209,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -1245,9 +1245,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1471320</xdr:colOff>
+      <xdr:colOff>1470960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1256,8 +1256,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3250080" y="4295160"/>
-          <a:ext cx="7835760" cy="2239560"/>
+          <a:off x="3250800" y="4295520"/>
+          <a:ext cx="7836480" cy="2239200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1279,7 +1279,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1522,9 +1522,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>162720</xdr:colOff>
+      <xdr:colOff>162360</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1538,12 +1538,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2746440" cy="2524680"/>
+          <a:ext cx="2746800" cy="2524320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1564,9 +1564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1471320</xdr:colOff>
+      <xdr:colOff>1470960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1575,8 +1575,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3250080" y="4295160"/>
-          <a:ext cx="7835760" cy="2239560"/>
+          <a:off x="3250800" y="4295520"/>
+          <a:ext cx="7836480" cy="2239200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1598,7 +1598,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1841,9 +1841,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>162720</xdr:colOff>
+      <xdr:colOff>162360</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1857,12 +1857,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2746440" cy="2524680"/>
+          <a:ext cx="2746800" cy="2524320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1883,9 +1883,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1471320</xdr:colOff>
+      <xdr:colOff>1470960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1894,8 +1894,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3250080" y="4295160"/>
-          <a:ext cx="7835760" cy="2239560"/>
+          <a:off x="3250800" y="4295520"/>
+          <a:ext cx="7836480" cy="2239200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1917,7 +1917,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -2160,9 +2160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>162720</xdr:colOff>
+      <xdr:colOff>162360</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2176,12 +2176,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2746440" cy="2524680"/>
+          <a:ext cx="2746800" cy="2524320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2203,10 +2203,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -2900,71 +2900,75 @@
     <mergeCell ref="W4:AB4"/>
     <mergeCell ref="AC4:AE4"/>
   </mergeCells>
-  <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 V6:V14 R7:U14" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:V14 S7:U14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+      <formula1>"Manual,Automatic"</formula1>
+      <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2986,10 +2990,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -3684,78 +3688,78 @@
     <mergeCell ref="AC4:AE4"/>
   </mergeCells>
   <dataValidations count="17">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
       <formula1>"Manual,Automatic"</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:V14" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:V14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
-      <formula1>"True,False"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
-      <formula1>-0.1</formula1>
-      <formula2>8</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3780,7 +3784,7 @@
       <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -4474,71 +4478,75 @@
     <mergeCell ref="W4:AB4"/>
     <mergeCell ref="AC4:AE4"/>
   </mergeCells>
-  <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 V6:V14 R7:U14" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:V14 S7:U14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+      <formula1>"Manual,Automatic"</formula1>
+      <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4559,7 +4567,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -4685,7 +4693,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
add full control of sample X/Y, slits W/H to all spreadsheets
+ fully deprecate e0 column
+ remove single wheel spreadsheet, use doublewheel for all wheels
+ linkam and lakeshore default to "element + temp at beginning" for filenames
+ change position of detector X column in all spreadsheets to be more left-ward

CAUTION! all of this fully breaks old spreadsheets
</commit_message>
<xml_diff>
--- a/startup/xlsx/glancing_angle.xlsx
+++ b/startup/xlsx/glancing_angle.xlsx
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S6" authorId="0">
+    <comment ref="R6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,6 +110,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="W6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -146,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S6" authorId="0">
+    <comment ref="R6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -202,6 +216,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="W6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -238,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S6" authorId="0">
+    <comment ref="R6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -294,12 +322,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="W6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="76">
   <si>
     <t xml:space="preserve">Glancing angle</t>
   </si>
@@ -307,21 +349,18 @@
     <t xml:space="preserve">Experimenters:</t>
   </si>
   <si>
-    <t xml:space="preserve">Change edge at start?</t>
+    <t xml:space="preserve">Close shutter at end?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add element to filename?</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">Close shutter at end?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add element to filename?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of repetitions</t>
   </si>
   <si>
@@ -401,6 +440,9 @@
   </si>
   <si>
     <t xml:space="preserve">Integration times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detector X</t>
   </si>
   <si>
     <t xml:space="preserve">Alignment method</t>
@@ -439,10 +481,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Slit height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detector X</t>
+    <t xml:space="preserve">Slit width (absolute width, mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slit height (absolute height, mm)</t>
   </si>
   <si>
     <t xml:space="preserve">snapshots</t>
@@ -554,6 +596,9 @@
   </si>
   <si>
     <t xml:space="preserve">added orientation and retraction distance to glancing angle spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add columns for sample X/Y + slit W/H to all spreadsheet types, also remove “Change edge at start?” + deprecate e0 column + deprecate single wheel spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -676,7 +721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -878,6 +923,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="true" diagonalDown="true">
+      <left style="thin"/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal style="medium"/>
+    </border>
+    <border diagonalUp="true" diagonalDown="true">
       <left style="thin">
         <color rgb="FFCCCCCC"/>
       </left>
@@ -927,7 +983,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1128,11 +1184,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1148,7 +1208,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1184,6 +1244,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1206,6 +1270,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1287,13 +1355,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>111600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1306,8 +1374,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4312800"/>
-          <a:ext cx="2746800" cy="2523960"/>
+          <a:off x="0" y="4313160"/>
+          <a:ext cx="2748600" cy="2522520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1328,9 +1396,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1925280</xdr:colOff>
+      <xdr:colOff>1923840</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1339,8 +1407,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3558240" y="4434480"/>
-          <a:ext cx="7985160" cy="2238480"/>
+          <a:off x="3561120" y="4434480"/>
+          <a:ext cx="7990560" cy="2237040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1417,16 +1485,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>2. Orientation (cell G3): para = sample surface parallel to X-ray electric vector / perp = </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>perpendicular</a:t>
+            <a:t>2. Orientation (cell G3): para = sample surface parallel to X-ray electric vector / perp = perpendicular</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1502,7 +1561,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>6. Specify pitch and y motor positions and the method for finding them in columns R, S, T</a:t>
+            <a:t>6. Specify pitch and y motor positions and the method for finding them in columns S, T, U</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1521,7 +1580,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. If column R is “Manual”, columns S and T </a:t>
+            <a:t>7. If column S is “Manual”, columns T and U </a:t>
           </a:r>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -1558,7 +1617,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>8. Specify detector position in column U, blank means to </a:t>
+            <a:t>8. Specify detector position in column R, blank means to </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -1614,7 +1673,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>10. Do not add columns before column AE</a:t>
+            <a:t>10. Do not add columns before column AG</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1638,9 +1697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1654,7 +1713,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2746800" cy="2523960"/>
+          <a:ext cx="2748600" cy="2522520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1668,16 +1727,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>303840</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33480</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1255680</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:colOff>1698480</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1686,8 +1745,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2888640" y="4192920"/>
-          <a:ext cx="7985160" cy="2238480"/>
+          <a:off x="3335760" y="4371840"/>
+          <a:ext cx="7990560" cy="2237040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1764,16 +1823,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>2. Orientation (cell G3): para = sample surface parallel to X-ray electric vector / perp = </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>perpendicular</a:t>
+            <a:t>2. Orientation (cell G3): para = sample surface parallel to X-ray electric vector / perp = perpendicular</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1849,7 +1899,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>6. Specify pitch and y motor positions and the method for finding them in columns R, S, T</a:t>
+            <a:t>6. Specify pitch and y motor positions and the method for finding them in columns S, T, U</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1868,7 +1918,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. If column R is “Manual”, columns S and T </a:t>
+            <a:t>7. If column S is “Manual”, columns T and U </a:t>
           </a:r>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -1905,7 +1955,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>8. Specify detector position in column U, blank means to </a:t>
+            <a:t>8. Specify detector position in column R, blank means to </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -1961,7 +2011,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>10. Do not add columns before column AE</a:t>
+            <a:t>10. Do not add columns before column AG</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1985,9 +2035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2001,7 +2051,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2746800" cy="2523960"/>
+          <a:ext cx="2748600" cy="2522520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2016,15 +2066,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>678600</xdr:colOff>
+      <xdr:colOff>707400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1630440</xdr:colOff>
+      <xdr:colOff>1658160</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2033,8 +2083,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3263400" y="4296600"/>
-          <a:ext cx="7985160" cy="2238480"/>
+          <a:off x="3295440" y="4327560"/>
+          <a:ext cx="7990560" cy="2237040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2073,17 +2123,7 @@
               <a:uFillTx/>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>Instructio</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFillTx/>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>ns:</a:t>
+            <a:t>Instructions:</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2102,52 +2142,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>1. Add the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>names of all </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>team </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>members to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>the green </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>box in row 1</a:t>
+            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2166,106 +2161,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>2. </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>Orientation </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>(cell G3): </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>para = </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>sample </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>surface </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>parallel to X-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>ray electric </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>vector / </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>perp = </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>perpendicul</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>ar</a:t>
+            <a:t>2. Orientation (cell G3): para = sample surface parallel to X-ray electric vector / perp = perpendicular</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2284,43 +2180,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>3. Default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>values for </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>all </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>parameters </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>go in line 6</a:t>
+            <a:t>3. Default values for all parameters go in line 6</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2339,43 +2199,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>4. Sample-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>specific </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>parameters </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>are entered </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>in rows 7+</a:t>
+            <a:t>4. Sample-specific parameters are entered in rows 7+</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2394,61 +2218,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>5. Default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>values from </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>line 6 will be </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>used for all </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>cells left </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>blank in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>rows 7+</a:t>
+            <a:t>5. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2467,79 +2237,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>6. Specify </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>pitch and y </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>motor </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>positions </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>and the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>method for </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>finding them </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>in columns </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>R, S, T</a:t>
+            <a:t>6. Specify pitch and y motor positions and the method for finding them in columns S, T, U</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2558,43 +2256,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. If column </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>R is </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>“Manual”, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>columns S </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>and T </a:t>
+            <a:t>7. If column S is “Manual”, columns T and U </a:t>
           </a:r>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -2612,16 +2274,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>be filled in</a:t>
+            <a:t> be filled in</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2640,52 +2293,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>8. Specify </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>detector </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>position in </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>column U, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>blank </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>means to </a:t>
+            <a:t>8. Specify detector position in column R, blank means to </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -2703,16 +2311,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>detector</a:t>
+            <a:t> detector</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2731,25 +2330,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>9. Do not </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>add rows </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>above row 7</a:t>
+            <a:t>9. Do not add rows above row 7</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2768,43 +2349,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>10. Do not </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>add </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>columns </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>before </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Bitstream Vera Sans"/>
-            </a:rPr>
-            <a:t>column AE</a:t>
+            <a:t>10. Do not add columns before column AG</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -2822,17 +2367,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AE38"/>
+  <dimension ref="B1:AF38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -2844,14 +2389,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="23" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="24" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2886,35 +2431,29 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 12</v>
+        <v>Version: 13</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="N2" s="10" t="n">
         <v>1</v>
@@ -2926,22 +2465,23 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="0"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
       <c r="AA2" s="0"/>
-      <c r="AB2" s="12"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="E3" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
@@ -2949,7 +2489,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="16"/>
       <c r="M3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N3" s="10" t="n">
         <v>10</v>
@@ -2961,26 +2501,27 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="0"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="12"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
       <c r="AA3" s="0"/>
-      <c r="AB3" s="12"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -2988,126 +2529,130 @@
         <v>0</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
       <c r="O4" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
       <c r="R4" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="21"/>
-      <c r="W4" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="X4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
       <c r="AB4" s="21"/>
-      <c r="AC4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD4" s="22"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="H5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="J5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="K5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="L5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="M5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="N5" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="O5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="30" t="s">
+      <c r="P5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="31" t="s">
+      <c r="R5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="S5" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="T5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="25" t="str">
+      <c r="U5" s="25" t="str">
         <f aca="false">IF(G3="para","Sample y abs. pos. (mm)","Sample x abs. pos. (mm)")</f>
         <v>Sample y abs. pos. (mm)</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="V5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="W5" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="W5" s="24" t="s">
+      <c r="X5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="X5" s="23" t="s">
+      <c r="Y5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="Z5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="AA5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AA5" s="23" t="s">
+      <c r="AB5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AC5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="AC5" s="27" t="s">
+      <c r="AD5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AD5" s="34" t="s">
+      <c r="AE5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="AE5" s="34" t="s">
+      <c r="AF5" s="34" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3116,7 +2661,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>48</v>
@@ -3128,7 +2673,7 @@
         <v>49</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" s="41" t="s">
         <v>50</v>
@@ -3160,375 +2705,383 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="50" t="s">
+      <c r="R6" s="50"/>
+      <c r="S6" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="52" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T6" s="52"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
       <c r="X6" s="53" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Y6" s="53" t="n">
+      <c r="Y6" s="54" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="54" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="53" t="n">
+      <c r="AA6" s="54" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="53" t="n">
+      <c r="AB6" s="54" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AB6" s="54" t="n">
+      <c r="AC6" s="55" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="55"/>
-      <c r="AD6" s="49"/>
+      <c r="AD6" s="56"/>
       <c r="AE6" s="49"/>
+      <c r="AF6" s="49"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="56" t="n">
+      <c r="B7" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="58"/>
+      <c r="C7" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="62"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="63"/>
       <c r="P7" s="35"/>
-      <c r="Q7" s="63"/>
-      <c r="T7" s="11"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="65"/>
       <c r="U7" s="11"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="68"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="70"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="56" t="n">
+      <c r="B8" s="57" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="58"/>
+      <c r="C8" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="59"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="62"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="63"/>
       <c r="P8" s="35"/>
-      <c r="Q8" s="63"/>
-      <c r="T8" s="11"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="65"/>
       <c r="U8" s="11"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="65"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="68"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="66"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="68"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="70"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="56" t="n">
+      <c r="B9" s="57" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="57" t="s">
-        <v>5</v>
+      <c r="C9" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="62"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="63"/>
       <c r="P9" s="35"/>
-      <c r="Q9" s="63"/>
-      <c r="T9" s="11"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="65"/>
       <c r="U9" s="11"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="68"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="70"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="56" t="n">
+      <c r="B10" s="57" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="57" t="s">
-        <v>5</v>
+      <c r="C10" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="62"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="63"/>
       <c r="P10" s="35"/>
-      <c r="Q10" s="63"/>
-      <c r="T10" s="11"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="65"/>
       <c r="U10" s="11"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="70"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="56" t="n">
+      <c r="B11" s="57" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>5</v>
+      <c r="C11" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="62"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="63"/>
       <c r="P11" s="35"/>
-      <c r="Q11" s="63"/>
-      <c r="T11" s="11"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="65"/>
       <c r="U11" s="11"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="65"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="68"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="67"/>
+      <c r="Y11" s="68"/>
+      <c r="Z11" s="68"/>
+      <c r="AA11" s="68"/>
+      <c r="AB11" s="68"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="70"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="56" t="n">
+      <c r="B12" s="57" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>5</v>
+      <c r="C12" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="62"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="63"/>
       <c r="P12" s="35"/>
-      <c r="Q12" s="63"/>
-      <c r="T12" s="11"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="65"/>
       <c r="U12" s="11"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="65"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="68"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="68"/>
+      <c r="Z12" s="68"/>
+      <c r="AA12" s="68"/>
+      <c r="AB12" s="68"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="70"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="56" t="n">
+      <c r="B13" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>5</v>
+      <c r="C13" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="62"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="63"/>
       <c r="P13" s="35"/>
-      <c r="Q13" s="63"/>
-      <c r="T13" s="11"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="65"/>
       <c r="U13" s="11"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="65"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="66"/>
-      <c r="Z13" s="66"/>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="68"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="67"/>
+      <c r="Y13" s="68"/>
+      <c r="Z13" s="68"/>
+      <c r="AA13" s="68"/>
+      <c r="AB13" s="68"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="70"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="56" t="n">
+      <c r="B14" s="57" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="57" t="s">
-        <v>5</v>
+      <c r="C14" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="62"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="63"/>
       <c r="P14" s="35"/>
-      <c r="Q14" s="63"/>
-      <c r="T14" s="11"/>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="65"/>
       <c r="U14" s="11"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="65"/>
-      <c r="X14" s="66"/>
-      <c r="Y14" s="66"/>
-      <c r="Z14" s="66"/>
-      <c r="AA14" s="66"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="67"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="68"/>
+      <c r="AA14" s="68"/>
+      <c r="AB14" s="68"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="70"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="56"/>
+      <c r="B21" s="57"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="56"/>
+      <c r="B22" s="57"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="56"/>
+      <c r="B23" s="57"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="56"/>
+      <c r="B24" s="57"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="56"/>
+      <c r="B25" s="57"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="56"/>
+      <c r="B26" s="57"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="56"/>
+      <c r="B27" s="57"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="56"/>
+      <c r="B28" s="57"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="56"/>
+      <c r="B29" s="57"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="56"/>
+      <c r="B30" s="57"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="56"/>
+      <c r="B31" s="57"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="56"/>
+      <c r="B32" s="57"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="56"/>
+      <c r="B33" s="57"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="56"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="56"/>
+      <c r="B35" s="57"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="56"/>
+      <c r="B36" s="57"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="56"/>
+      <c r="B37" s="57"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="56"/>
+      <c r="B38" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:AB1"/>
+    <mergeCell ref="E1:AC1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C4:D4"/>
@@ -3536,12 +3089,12 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="R4:W4"/>
+    <mergeCell ref="X4:AC4"/>
+    <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
+  <dataValidations count="18">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3557,7 +3110,7 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3585,29 +3138,33 @@
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:V14 S7:U14" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 T7:W14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S14" type="list">
       <formula1>"Manual,Automatic"</formula1>
       <formula2>150</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G3" type="list">
       <formula1>"para,perp"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3627,17 +3184,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AE38"/>
+  <dimension ref="B1:AF38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -3649,14 +3206,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="23" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="24" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3691,35 +3248,29 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 12</v>
+        <v>Version: 13</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="N2" s="10" t="n">
         <v>1</v>
@@ -3731,22 +3282,23 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="0"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
       <c r="AA2" s="0"/>
-      <c r="AB2" s="12"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="E3" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
@@ -3754,7 +3306,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="16"/>
       <c r="M3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N3" s="10" t="n">
         <v>10</v>
@@ -3766,26 +3318,27 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="0"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="12"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
       <c r="AA3" s="0"/>
-      <c r="AB3" s="12"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -3793,126 +3346,130 @@
         <v>0</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
       <c r="O4" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
       <c r="R4" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="21"/>
-      <c r="W4" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="X4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
       <c r="AB4" s="21"/>
-      <c r="AC4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD4" s="22"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="H5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="J5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="K5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="L5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="M5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="N5" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="O5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="30" t="s">
+      <c r="P5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="31" t="s">
+      <c r="R5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="S5" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="T5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="25" t="str">
+      <c r="U5" s="25" t="str">
         <f aca="false">IF(G3="para","Sample y abs. pos. (mm)","Sample x abs. pos. (mm)")</f>
         <v>Sample y abs. pos. (mm)</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="V5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="W5" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="W5" s="24" t="s">
+      <c r="X5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="X5" s="23" t="s">
+      <c r="Y5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="Z5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="AA5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AA5" s="23" t="s">
+      <c r="AB5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AC5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="AC5" s="27" t="s">
+      <c r="AD5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AD5" s="34" t="s">
+      <c r="AE5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="AE5" s="34" t="s">
+      <c r="AF5" s="34" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3921,7 +3478,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>48</v>
@@ -3933,7 +3490,7 @@
         <v>49</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" s="41" t="s">
         <v>50</v>
@@ -3965,375 +3522,383 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="50" t="s">
+      <c r="R6" s="50"/>
+      <c r="S6" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="52" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T6" s="52"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
       <c r="X6" s="53" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Y6" s="53" t="n">
+      <c r="Y6" s="54" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="54" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="53" t="n">
+      <c r="AA6" s="54" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="53" t="n">
+      <c r="AB6" s="54" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AB6" s="54" t="n">
+      <c r="AC6" s="55" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="55"/>
-      <c r="AD6" s="49"/>
+      <c r="AD6" s="56"/>
       <c r="AE6" s="49"/>
+      <c r="AF6" s="49"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="56" t="n">
+      <c r="B7" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="58"/>
+      <c r="C7" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="62"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="63"/>
       <c r="P7" s="35"/>
-      <c r="Q7" s="63"/>
-      <c r="T7" s="11"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="65"/>
       <c r="U7" s="11"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="68"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="70"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="56" t="n">
+      <c r="B8" s="57" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="58"/>
+      <c r="C8" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="59"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="62"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="63"/>
       <c r="P8" s="35"/>
-      <c r="Q8" s="63"/>
-      <c r="T8" s="11"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="65"/>
       <c r="U8" s="11"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="65"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="68"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="66"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="68"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="70"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="56" t="n">
+      <c r="B9" s="57" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="57" t="s">
-        <v>5</v>
+      <c r="C9" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="62"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="63"/>
       <c r="P9" s="35"/>
-      <c r="Q9" s="63"/>
-      <c r="T9" s="11"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="65"/>
       <c r="U9" s="11"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="68"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="70"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="56" t="n">
+      <c r="B10" s="57" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="57" t="s">
-        <v>5</v>
+      <c r="C10" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="62"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="63"/>
       <c r="P10" s="35"/>
-      <c r="Q10" s="63"/>
-      <c r="T10" s="11"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="65"/>
       <c r="U10" s="11"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="70"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="56" t="n">
+      <c r="B11" s="57" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>5</v>
+      <c r="C11" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="62"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="63"/>
       <c r="P11" s="35"/>
-      <c r="Q11" s="63"/>
-      <c r="T11" s="11"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="65"/>
       <c r="U11" s="11"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="65"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="68"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="67"/>
+      <c r="Y11" s="68"/>
+      <c r="Z11" s="68"/>
+      <c r="AA11" s="68"/>
+      <c r="AB11" s="68"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="70"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="56" t="n">
+      <c r="B12" s="57" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>5</v>
+      <c r="C12" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="62"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="63"/>
       <c r="P12" s="35"/>
-      <c r="Q12" s="63"/>
-      <c r="T12" s="11"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="65"/>
       <c r="U12" s="11"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="65"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="68"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="68"/>
+      <c r="Z12" s="68"/>
+      <c r="AA12" s="68"/>
+      <c r="AB12" s="68"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="70"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="56" t="n">
+      <c r="B13" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>5</v>
+      <c r="C13" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="62"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="63"/>
       <c r="P13" s="35"/>
-      <c r="Q13" s="63"/>
-      <c r="T13" s="11"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="65"/>
       <c r="U13" s="11"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="65"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="66"/>
-      <c r="Z13" s="66"/>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="68"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="67"/>
+      <c r="Y13" s="68"/>
+      <c r="Z13" s="68"/>
+      <c r="AA13" s="68"/>
+      <c r="AB13" s="68"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="70"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="56" t="n">
+      <c r="B14" s="57" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="57" t="s">
-        <v>5</v>
+      <c r="C14" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="62"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="63"/>
       <c r="P14" s="35"/>
-      <c r="Q14" s="63"/>
-      <c r="T14" s="11"/>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="65"/>
       <c r="U14" s="11"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="65"/>
-      <c r="X14" s="66"/>
-      <c r="Y14" s="66"/>
-      <c r="Z14" s="66"/>
-      <c r="AA14" s="66"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="67"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="68"/>
+      <c r="AA14" s="68"/>
+      <c r="AB14" s="68"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="70"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="56"/>
+      <c r="B21" s="57"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="56"/>
+      <c r="B22" s="57"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="56"/>
+      <c r="B23" s="57"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="56"/>
+      <c r="B24" s="57"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="56"/>
+      <c r="B25" s="57"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="56"/>
+      <c r="B26" s="57"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="56"/>
+      <c r="B27" s="57"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="56"/>
+      <c r="B28" s="57"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="56"/>
+      <c r="B29" s="57"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="56"/>
+      <c r="B30" s="57"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="56"/>
+      <c r="B31" s="57"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="56"/>
+      <c r="B32" s="57"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="56"/>
+      <c r="B33" s="57"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="56"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="56"/>
+      <c r="B35" s="57"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="56"/>
+      <c r="B36" s="57"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="56"/>
+      <c r="B37" s="57"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="56"/>
+      <c r="B38" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:AB1"/>
+    <mergeCell ref="E1:AC1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C4:D4"/>
@@ -4341,12 +3906,12 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="R4:W4"/>
+    <mergeCell ref="X4:AC4"/>
+    <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="18">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
+  <dataValidations count="19">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4362,7 +3927,7 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4390,33 +3955,37 @@
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S14" type="list">
       <formula1>"Manual,Automatic"</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:V14" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G3" type="list">
       <formula1>"para,perp"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:W14" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4436,17 +4005,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AE38"/>
+  <dimension ref="B1:AF38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -4458,14 +4027,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="23" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="24" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4500,35 +4069,29 @@
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 12</v>
+        <v>Version: 13</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="N2" s="10" t="n">
         <v>1</v>
@@ -4540,22 +4103,23 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="0"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
       <c r="AA2" s="0"/>
-      <c r="AB2" s="12"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="E3" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
@@ -4563,7 +4127,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="16"/>
       <c r="M3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N3" s="10" t="n">
         <v>10</v>
@@ -4575,26 +4139,27 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
       <c r="V3" s="11"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="0"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="12"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
       <c r="AA3" s="0"/>
-      <c r="AB3" s="12"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -4602,126 +4167,130 @@
         <v>0</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
       <c r="O4" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
       <c r="R4" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="21"/>
-      <c r="W4" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="X4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
       <c r="AA4" s="21"/>
       <c r="AB4" s="21"/>
-      <c r="AC4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD4" s="22"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="22" t="s">
+        <v>17</v>
+      </c>
       <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="H5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="J5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="K5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="L5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="M5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="N5" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="O5" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="30" t="s">
+      <c r="P5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="Q5" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="31" t="s">
+      <c r="R5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="S5" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="T5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="25" t="str">
+      <c r="U5" s="25" t="str">
         <f aca="false">IF(G3="para","Sample y abs. pos. (mm)","Sample x abs. pos. (mm)")</f>
         <v>Sample y abs. pos. (mm)</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="V5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="V5" s="25" t="s">
+      <c r="W5" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="W5" s="24" t="s">
+      <c r="X5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="X5" s="23" t="s">
+      <c r="Y5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="Z5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="AA5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="AA5" s="23" t="s">
+      <c r="AB5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AC5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="AC5" s="27" t="s">
+      <c r="AD5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AD5" s="34" t="s">
+      <c r="AE5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="AE5" s="34" t="s">
+      <c r="AF5" s="34" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4730,7 +4299,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>48</v>
@@ -4742,7 +4311,7 @@
         <v>49</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H6" s="41" t="s">
         <v>50</v>
@@ -4774,375 +4343,383 @@
       <c r="Q6" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="50" t="s">
+      <c r="R6" s="50"/>
+      <c r="S6" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="52" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T6" s="52"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
       <c r="X6" s="53" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Y6" s="53" t="n">
+      <c r="Y6" s="54" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Z6" s="54" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="53" t="n">
+      <c r="AA6" s="54" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="53" t="n">
+      <c r="AB6" s="54" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AB6" s="54" t="n">
+      <c r="AC6" s="55" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="55"/>
-      <c r="AD6" s="49"/>
+      <c r="AD6" s="56"/>
       <c r="AE6" s="49"/>
+      <c r="AF6" s="49"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="56" t="n">
+      <c r="B7" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="58"/>
+      <c r="C7" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="62"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="63"/>
       <c r="P7" s="35"/>
-      <c r="Q7" s="63"/>
-      <c r="T7" s="11"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="65"/>
       <c r="U7" s="11"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="67"/>
-      <c r="AC7" s="68"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="70"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="56" t="n">
+      <c r="B8" s="57" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="58"/>
+      <c r="C8" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="59"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="62"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="63"/>
       <c r="P8" s="35"/>
-      <c r="Q8" s="63"/>
-      <c r="T8" s="11"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="65"/>
       <c r="U8" s="11"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="65"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="67"/>
-      <c r="AC8" s="68"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="66"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="68"/>
+      <c r="Z8" s="68"/>
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="69"/>
+      <c r="AD8" s="70"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="56" t="n">
+      <c r="B9" s="57" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="57" t="s">
-        <v>5</v>
+      <c r="C9" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="62"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="63"/>
       <c r="P9" s="35"/>
-      <c r="Q9" s="63"/>
-      <c r="T9" s="11"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="65"/>
       <c r="U9" s="11"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="66"/>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="67"/>
-      <c r="AC9" s="68"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="67"/>
+      <c r="Y9" s="68"/>
+      <c r="Z9" s="68"/>
+      <c r="AA9" s="68"/>
+      <c r="AB9" s="68"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="70"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="56" t="n">
+      <c r="B10" s="57" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="57" t="s">
-        <v>5</v>
+      <c r="C10" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="62"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="63"/>
       <c r="P10" s="35"/>
-      <c r="Q10" s="63"/>
-      <c r="T10" s="11"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="65"/>
       <c r="U10" s="11"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="66"/>
-      <c r="Z10" s="66"/>
-      <c r="AA10" s="66"/>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="68"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="67"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="70"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="56" t="n">
+      <c r="B11" s="57" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="57" t="s">
-        <v>5</v>
+      <c r="C11" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="62"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="63"/>
       <c r="P11" s="35"/>
-      <c r="Q11" s="63"/>
-      <c r="T11" s="11"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="65"/>
       <c r="U11" s="11"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="65"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="66"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="68"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="67"/>
+      <c r="Y11" s="68"/>
+      <c r="Z11" s="68"/>
+      <c r="AA11" s="68"/>
+      <c r="AB11" s="68"/>
+      <c r="AC11" s="69"/>
+      <c r="AD11" s="70"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="56" t="n">
+      <c r="B12" s="57" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>5</v>
+      <c r="C12" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="63"/>
-      <c r="O12" s="62"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="63"/>
       <c r="P12" s="35"/>
-      <c r="Q12" s="63"/>
-      <c r="T12" s="11"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="65"/>
       <c r="U12" s="11"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="65"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="66"/>
-      <c r="Z12" s="66"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="68"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="68"/>
+      <c r="Z12" s="68"/>
+      <c r="AA12" s="68"/>
+      <c r="AB12" s="68"/>
+      <c r="AC12" s="69"/>
+      <c r="AD12" s="70"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="56" t="n">
+      <c r="B13" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>5</v>
+      <c r="C13" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="62"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="63"/>
       <c r="P13" s="35"/>
-      <c r="Q13" s="63"/>
-      <c r="T13" s="11"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="65"/>
       <c r="U13" s="11"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="65"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="66"/>
-      <c r="Z13" s="66"/>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="68"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="67"/>
+      <c r="Y13" s="68"/>
+      <c r="Z13" s="68"/>
+      <c r="AA13" s="68"/>
+      <c r="AB13" s="68"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="70"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="56" t="n">
+      <c r="B14" s="57" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="57" t="s">
-        <v>5</v>
+      <c r="C14" s="58" t="s">
+        <v>3</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="63"/>
-      <c r="O14" s="62"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="63"/>
       <c r="P14" s="35"/>
-      <c r="Q14" s="63"/>
-      <c r="T14" s="11"/>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="65"/>
       <c r="U14" s="11"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="65"/>
-      <c r="X14" s="66"/>
-      <c r="Y14" s="66"/>
-      <c r="Z14" s="66"/>
-      <c r="AA14" s="66"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="66"/>
+      <c r="X14" s="67"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="68"/>
+      <c r="AA14" s="68"/>
+      <c r="AB14" s="68"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="70"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="56"/>
+      <c r="B21" s="57"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="56"/>
+      <c r="B22" s="57"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="56"/>
+      <c r="B23" s="57"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="56"/>
+      <c r="B24" s="57"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="56"/>
+      <c r="B25" s="57"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="56"/>
+      <c r="B26" s="57"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="56"/>
+      <c r="B27" s="57"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="56"/>
+      <c r="B28" s="57"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="56"/>
+      <c r="B29" s="57"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="56"/>
+      <c r="B30" s="57"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="56"/>
+      <c r="B31" s="57"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="56"/>
+      <c r="B32" s="57"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="56"/>
+      <c r="B33" s="57"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="56"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="56"/>
+      <c r="B35" s="57"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="56"/>
+      <c r="B36" s="57"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="56"/>
+      <c r="B37" s="57"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="56"/>
+      <c r="B38" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:AB1"/>
+    <mergeCell ref="E1:AC1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C4:D4"/>
@@ -5150,12 +4727,12 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:V4"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="R4:W4"/>
+    <mergeCell ref="X4:AC4"/>
+    <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:AB14" type="list">
+  <dataValidations count="18">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5171,7 +4748,7 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5199,29 +4776,33 @@
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W6:AB6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AC6:AE6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:V14 S7:U14" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 T7:W14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S14" type="list">
       <formula1>"Manual,Automatic"</formula1>
       <formula2>150</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G3" type="list">
       <formula1>"para,perp"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5241,19 +4822,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
   </cols>
   <sheetData>
-    <row r="1" s="69" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="71" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
         <v>60</v>
       </c>
@@ -5262,23 +4843,23 @@
       <c r="A2" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="71"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="n">
-        <v>12</v>
-      </c>
-      <c r="B3" s="69"/>
+        <v>13</v>
+      </c>
+      <c r="B3" s="71"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="34"/>
-      <c r="B4" s="69"/>
+      <c r="B4" s="71"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="71" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5376,6 +4957,14 @@
       </c>
       <c r="B17" s="0" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>